<commit_message>
spreadsheet and picture upload
</commit_message>
<xml_diff>
--- a/spreadsheets/Ahri.xlsx
+++ b/spreadsheets/Ahri.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\champsgg\completed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992D609A-5E7F-4C6D-BD05-F47002463552}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55043A57-C9AD-41AF-ADA1-14B6659403E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -295,15 +295,9 @@
     <t>description/bio</t>
   </si>
   <si>
-    <t>Ambitieux is a Diamond 1 Ahri player. Is known for a very aggressive playstyle. High risk high reward. Highest peak was Diamond 1. 90 LP. (Also at one point was 2nd Ahri in NA)</t>
-  </si>
-  <si>
     <t>extra message</t>
   </si>
   <si>
-    <t>Follow Ambitieux if you want solid content, while picking up some knowledge on Ahri in the mid lane</t>
-  </si>
-  <si>
     <t>After the site launches, any of this information can be changed.</t>
   </si>
   <si>
@@ -407,6 +401,12 @@
   </si>
   <si>
     <t>https://i.imgur.com/uvW6E8o.png</t>
+  </si>
+  <si>
+    <t>Ambitieux is a Diamond 1 Ahri player. Is known for a very aggressive playstyle. High risk high reward. Highest peak was Diamond 1. 90 LP. Also at one point was 2nd best Ahri in NA.</t>
+  </si>
+  <si>
+    <t>Follow Ambitieux if you want solid content, while picking up some knowledge on Ahri in the mid lane.</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -873,7 +873,7 @@
         <v>86</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>87</v>
@@ -884,32 +884,32 @@
         <v>88</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1942,7 +1942,7 @@
         <v>4.5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1954,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1966,7 +1966,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -1978,7 +1978,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -1990,7 +1990,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -2014,7 +2014,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2048,7 +2048,7 @@
         <v>7.5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>4.5</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>8.5</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2169,7 @@
         <v>3.5</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2257,7 +2257,7 @@
         <v>8</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
         <v>3.5</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
         <v>6.5</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
         <v>6</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>8</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2433,7 +2433,7 @@
         <v>6.5</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>